<commit_message>
AJ: Added links to MSc thesis of Glinserer and Baischer.
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="793">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2624,6 +2624,9 @@
     <t xml:space="preserve">Autopruning  mit  Intel  Distiller  und  Evaluation  auf  einem  Jetson  Xavier AGX</t>
   </si>
   <si>
+    <t xml:space="preserve">https://doi.org/10.34726/hss.2021.90301</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marco Wuschnig</t>
   </si>
   <si>
@@ -2685,6 +2688,9 @@
   </si>
   <si>
     <t xml:space="preserve">FPGA Based Embedded Neural Network Object Detector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.34726/hss.2021.69314</t>
   </si>
   <si>
     <t xml:space="preserve">Embedded Machine Learning Scripts and Guides</t>
@@ -2898,15 +2904,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0\ %"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0"/>
-    <numFmt numFmtId="169" formatCode="dd/mmm"/>
+    <numFmt numFmtId="169" formatCode="DD/MMM"/>
     <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="General"/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -4916,7 +4921,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4936,7 +4941,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="12" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4948,7 +4953,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5020,7 +5025,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5108,7 +5113,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="13" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5132,11 +5137,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="14" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="15" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5144,7 +5149,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="16" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5188,7 +5193,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="69" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="69" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5266,14 +5271,14 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Standard 2" xfId="21"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Standard 2" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="1222">
     <dxf>
@@ -14693,7 +14698,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14707,7 +14712,7 @@
       <selection pane="bottomRight" activeCell="AZ117" activeCellId="0" sqref="AZ117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.11"/>
@@ -14727,22 +14732,22 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="4" width="3.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="38" min="32" style="2" width="3.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="39" min="39" style="5" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="40" min="40" style="5" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="40" min="40" style="5" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="41" min="41" style="6" width="7.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="6" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="7" width="38.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="8" width="41.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="8" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="8" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="8" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="7" width="35.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="7" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="7" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="7" width="47.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="7" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="7" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="7" width="47.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="7" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="7" width="52.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="7" width="72.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="8.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="55" style="1" width="11.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="55" style="1" width="11.44"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36761,7 +36766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -36771,17 +36776,19 @@
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="316" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B1" s="316" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36794,10 +36801,10 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36805,7 +36812,7 @@
         <v>128</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36813,7 +36820,7 @@
         <v>177</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36821,7 +36828,7 @@
         <v>403</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36837,7 +36844,7 @@
         <v>90</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36861,7 +36868,7 @@
         <v>502</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36877,7 +36884,7 @@
         <v>329</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36893,7 +36900,7 @@
         <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36901,7 +36908,7 @@
         <v>147</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36922,10 +36929,10 @@
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36957,7 +36964,7 @@
         <v>620</v>
       </c>
       <c r="B23" s="317" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36965,7 +36972,7 @@
         <v>625</v>
       </c>
       <c r="B24" s="318" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36973,7 +36980,7 @@
         <v>629</v>
       </c>
       <c r="B25" s="318" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36984,7 +36991,7 @@
         <v>621</v>
       </c>
       <c r="B27" s="318" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36992,7 +36999,7 @@
         <v>626</v>
       </c>
       <c r="B28" s="318" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37000,7 +37007,7 @@
         <v>630</v>
       </c>
       <c r="B29" s="318" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37023,7 +37030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -37033,9 +37040,11 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37043,22 +37052,22 @@
         <v>10</v>
       </c>
       <c r="C1" s="319" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="H1" s="316" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="C2" s="320" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="H2" s="321" t="n">
         <f aca="true">TODAY()</f>
-        <v>44505</v>
+        <v>44586</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37066,15 +37075,15 @@
         <v>91</v>
       </c>
       <c r="C3" s="320" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="C4" s="320" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37082,7 +37091,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="320" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37090,32 +37099,32 @@
         <v>36</v>
       </c>
       <c r="C6" s="320" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="320" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="320" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="320" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="320" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="320" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
     </row>
   </sheetData>
@@ -37130,7 +37139,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -37140,14 +37149,15 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="54.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="24.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="10"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="230" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="230" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" s="233" customFormat="true" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38115,7 +38125,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -38125,7 +38135,7 @@
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="54.44"/>
@@ -38134,8 +38144,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="24.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="251" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="229" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="252" width="6.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="230" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="252" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="230" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" s="233" customFormat="true" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -39723,7 +39734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -39733,19 +39744,19 @@
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="32.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="32.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="250" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="251" width="8.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="251" width="8.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="229" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="271" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="229" width="45.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="229" width="43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="230" width="12.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="230" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="230" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" s="233" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -41678,7 +41689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -41688,7 +41699,7 @@
       <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="54.44"/>
@@ -41697,7 +41708,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="229" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="251" width="8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="230" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="230" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" s="233" customFormat="true" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43147,7 +43159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -43157,13 +43169,14 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="22.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="65.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="65.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="252" width="37.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43403,26 +43416,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="22.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="60.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="15.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="252" width="37.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="271" width="11.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="229" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="271" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="229" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" s="301" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43482,7 +43495,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="228" t="s">
         <v>677</v>
       </c>
@@ -43498,13 +43511,16 @@
       <c r="E4" s="229" t="n">
         <v>2021</v>
       </c>
+      <c r="F4" s="252" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="228" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B5" s="229" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C5" s="229" t="s">
         <v>674</v>
@@ -43516,15 +43532,15 @@
         <v>2020</v>
       </c>
       <c r="F5" s="306" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="228" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B6" s="229" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C6" s="229" t="s">
         <v>674</v>
@@ -43536,15 +43552,15 @@
         <v>2020</v>
       </c>
       <c r="F6" s="306" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="228" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B7" s="229" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C7" s="229" t="s">
         <v>679</v>
@@ -43556,15 +43572,15 @@
         <v>2021</v>
       </c>
       <c r="F7" s="306" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="228" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B8" s="229" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C8" s="229" t="s">
         <v>669</v>
@@ -43578,10 +43594,10 @@
     </row>
     <row r="9" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="228" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B9" s="229" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C9" s="229" t="s">
         <v>674</v>
@@ -43593,7 +43609,7 @@
         <v>2021</v>
       </c>
       <c r="F9" s="306" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43601,7 +43617,7 @@
         <v>675</v>
       </c>
       <c r="B10" s="307" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C10" s="229" t="s">
         <v>674</v>
@@ -43615,10 +43631,10 @@
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="228" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B11" s="307" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C11" s="229" t="s">
         <v>674</v>
@@ -43632,10 +43648,10 @@
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="228" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B12" s="229" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C12" s="229" t="s">
         <v>679</v>
@@ -43647,12 +43663,12 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="228" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B13" s="229" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C13" s="229" t="s">
         <v>679</v>
@@ -43662,6 +43678,9 @@
       </c>
       <c r="E13" s="229" t="n">
         <v>2021</v>
+      </c>
+      <c r="F13" s="252" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43690,7 +43709,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -43700,12 +43719,12 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="229" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="39.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="56.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="230" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="230" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" s="311" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43721,68 +43740,68 @@
     </row>
     <row r="2" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="248" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B2" s="249" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C2" s="312" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="228" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B3" s="229" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C3" s="306" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="228" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B4" s="229" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="C4" s="306" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="228" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B5" s="229" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="C5" s="306" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="228" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B6" s="229" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="C6" s="306" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="228" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B7" s="229" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="C7" s="306" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43855,7 +43874,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -43865,23 +43884,23 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="313" width="11.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="250" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="9.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="46.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="15.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="6" min="6" style="229" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="7" min="7" style="229" width="40"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="8" min="8" style="229" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="252" width="19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="230" width="11.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="230" width="11.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="314" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B1" s="315" t="s">
         <v>1</v>
@@ -43890,19 +43909,19 @@
         <v>665</v>
       </c>
       <c r="D1" s="301" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="E1" s="301" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="F1" s="301" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="301" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="H1" s="301" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="I1" s="302" t="s">
         <v>10</v>
@@ -43910,19 +43929,19 @@
     </row>
     <row r="2" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="229" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="D2" s="243" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="E2" s="243" t="s">
         <v>668</v>
       </c>
       <c r="G2" s="229" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="I2" s="252" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43930,19 +43949,19 @@
         <v>44153</v>
       </c>
       <c r="C3" s="229" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D3" s="243" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="E3" s="243" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="G3" s="243" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="I3" s="252" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43950,19 +43969,19 @@
         <v>44153</v>
       </c>
       <c r="C4" s="229" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="D4" s="243" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="E4" s="243" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="G4" s="243" t="s">
+        <v>757</v>
+      </c>
+      <c r="I4" s="252" t="s">
         <v>755</v>
-      </c>
-      <c r="I4" s="252" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43970,100 +43989,100 @@
         <v>44294</v>
       </c>
       <c r="C5" s="229" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="D5" s="229" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="E5" s="229" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="I5" s="252" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="229" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="D6" s="229" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="E6" s="229" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="I6" s="252" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="229" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D7" s="229" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="E7" s="229" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="I7" s="252" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="229" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D8" s="229" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="E8" s="229" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="I8" s="252" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="229" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D9" s="229" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="E9" s="229" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="I9" s="252" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="229" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D10" s="229" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="E10" s="229" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="I10" s="252" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="229" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="D11" s="229" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="E11" s="229" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="I11" s="252" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44071,16 +44090,16 @@
         <v>44294</v>
       </c>
       <c r="C12" s="229" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D12" s="229" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="E12" s="229" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="I12" s="252" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add opentheses to menu
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -2662,10 +2662,10 @@
     <t xml:space="preserve">https://github.com/embedded-machine-learning/MobileNetV3-Segmentation-Keras</t>
   </si>
   <si>
-    <t xml:space="preserve">Betreuer 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Betreuer 2</t>
+    <t xml:space="preserve">Supervisor 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervisor 2</t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
@@ -2683,13 +2683,13 @@
     <t xml:space="preserve">Wess</t>
   </si>
   <si>
-    <t xml:space="preserve">Anpassung eines Latenz- und Leistungsschätzungsmodell für ARM Prozessoren</t>
+    <t xml:space="preserve">Adaptation of a Latency and Power Estimation Model for ARM Processors</t>
   </si>
   <si>
     <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=9078&amp;dsrid=628&amp;thesisId=83155</t>
   </si>
   <si>
-    <t xml:space="preserve">Pruning von Slimmable Deep Neural Networks an einer Intel Neural Processing Unit</t>
+    <t xml:space="preserve">Energy Efficient Adaptive Neural Networks for Embedded Hardware</t>
   </si>
   <si>
     <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8615&amp;dsrid=533&amp;thesisId=89084</t>
@@ -2698,7 +2698,7 @@
     <t xml:space="preserve">DA</t>
   </si>
   <si>
-    <t xml:space="preserve">Power-Aware Pruning on Embedded Platforms with Reinforcement Learning</t>
+    <t xml:space="preserve">Adaptive Neural Network low bit-width Quantization for image classification, object detection and segmentation targeting FPGA</t>
   </si>
   <si>
     <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8461&amp;dsrid=505&amp;thesisId=89961</t>
@@ -2765,7 +2765,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0\ %"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
@@ -2774,7 +2774,6 @@
     <numFmt numFmtId="169" formatCode="dd/mmm"/>
     <numFmt numFmtId="170" formatCode="0.0000"/>
     <numFmt numFmtId="171" formatCode="General"/>
-    <numFmt numFmtId="172" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -4854,7 +4853,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4866,7 +4865,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -37802,8 +37801,8 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37853,7 +37852,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="264" t="s">
         <v>721</v>
       </c>
@@ -37864,16 +37863,16 @@
         <v>723</v>
       </c>
       <c r="D3" s="265" t="n">
-        <v>43621</v>
-      </c>
-      <c r="E3" s="266" t="s">
+        <v>44266</v>
+      </c>
+      <c r="E3" s="256" t="s">
         <v>726</v>
       </c>
       <c r="F3" s="264" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="264" t="s">
         <v>728</v>
       </c>
@@ -37884,9 +37883,9 @@
         <v>723</v>
       </c>
       <c r="D4" s="265" t="n">
-        <v>44562</v>
-      </c>
-      <c r="E4" s="266" t="s">
+        <v>44294</v>
+      </c>
+      <c r="E4" s="256" t="s">
         <v>729</v>
       </c>
       <c r="F4" s="264" t="s">
@@ -37904,7 +37903,7 @@
         <v>731</v>
       </c>
       <c r="D5" s="265" t="n">
-        <v>44562</v>
+        <v>44299</v>
       </c>
       <c r="E5" s="267" t="s">
         <v>732</v>
@@ -37924,7 +37923,7 @@
         <v>731</v>
       </c>
       <c r="D6" s="265" t="n">
-        <v>43621</v>
+        <v>44102</v>
       </c>
       <c r="E6" s="267" t="s">
         <v>734</v>
@@ -37964,7 +37963,7 @@
         <v>731</v>
       </c>
       <c r="D8" s="265" t="n">
-        <v>43621</v>
+        <v>44504</v>
       </c>
       <c r="E8" s="267" t="s">
         <v>738</v>
@@ -37984,7 +37983,7 @@
         <v>740</v>
       </c>
       <c r="D9" s="265" t="n">
-        <v>44562</v>
+        <v>44564</v>
       </c>
       <c r="E9" s="267" t="s">
         <v>741</v>
@@ -38004,7 +38003,7 @@
         <v>743</v>
       </c>
       <c r="D10" s="265" t="n">
-        <v>44562</v>
+        <v>42509</v>
       </c>
       <c r="E10" s="267" t="s">
         <v>744</v>
@@ -38021,7 +38020,7 @@
         <v>722</v>
       </c>
       <c r="D11" s="265" t="n">
-        <v>44562</v>
+        <v>43279</v>
       </c>
       <c r="E11" s="267" t="s">
         <v>746</v>
@@ -38038,7 +38037,7 @@
         <v>722</v>
       </c>
       <c r="D12" s="265" t="n">
-        <v>43621</v>
+        <v>43279</v>
       </c>
       <c r="E12" s="267" t="s">
         <v>748</v>

</xml_diff>

<commit_message>
Lukas Steindl in _/Data/CDLEML_WP_Progress_EML-Process.xlsx eingefügt
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EML_Tool_WP" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="753">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2606,6 +2606,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.34726/hss.2021.69314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lukas Steindl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimizing deep neural networks for efficient dronebased ragweed detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.34726/hss.2022.79705</t>
   </si>
   <si>
     <t xml:space="preserve">Embedded Machine Learning Scripts and Guides</t>
@@ -37340,8 +37349,8 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.56640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37603,6 +37612,32 @@
       <c r="F13" s="247" t="s">
         <v>698</v>
       </c>
+    </row>
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="256" t="s">
+        <v>699</v>
+      </c>
+      <c r="B14" s="256" t="s">
+        <v>700</v>
+      </c>
+      <c r="C14" s="229" t="s">
+        <v>665</v>
+      </c>
+      <c r="D14" s="229" t="s">
+        <v>671</v>
+      </c>
+      <c r="E14" s="229" t="n">
+        <v>2022</v>
+      </c>
+      <c r="F14" s="256" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="256"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="257"/>
@@ -37661,68 +37696,68 @@
     </row>
     <row r="2" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="245" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="B2" s="246" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="C2" s="262" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="228" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="B3" s="229" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="C3" s="255" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="228" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="B4" s="229" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="C4" s="255" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="228" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B5" s="229" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="C5" s="255" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="228" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="B6" s="229" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="C6" s="255" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="228" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="B7" s="229" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="C7" s="255" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37801,7 +37836,7 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -37817,16 +37852,16 @@
         <v>659</v>
       </c>
       <c r="B1" s="264" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="C1" s="264" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="D1" s="264" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="E1" s="264" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="F1" s="264" t="s">
         <v>662</v>
@@ -37834,216 +37869,216 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="264" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B2" s="264" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C2" s="264" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="D2" s="265" t="n">
         <v>44562</v>
       </c>
       <c r="E2" s="266" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="F2" s="264" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="264" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B3" s="264" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C3" s="264" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="D3" s="265" t="n">
         <v>44266</v>
       </c>
       <c r="E3" s="256" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="F3" s="264" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="264" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B4" s="264" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C4" s="264" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="D4" s="265" t="n">
         <v>44294</v>
       </c>
       <c r="E4" s="256" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="F4" s="264" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="D5" s="265" t="n">
         <v>44299</v>
       </c>
       <c r="E5" s="267" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="D6" s="265" t="n">
         <v>44102</v>
       </c>
       <c r="E6" s="267" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="D7" s="265" t="n">
         <v>44562</v>
       </c>
       <c r="E7" s="267" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="D8" s="265" t="n">
         <v>44504</v>
       </c>
       <c r="E8" s="267" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="D9" s="265" t="n">
         <v>44564</v>
       </c>
       <c r="E9" s="267" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="D10" s="265" t="n">
         <v>42509</v>
       </c>
       <c r="E10" s="267" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="D11" s="265" t="n">
         <v>43279</v>
       </c>
       <c r="E11" s="267" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="D12" s="265" t="n">
         <v>43279</v>
       </c>
       <c r="E12" s="267" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added Nikolas Alge's thesis in completed-list.
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="755">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2617,6 +2617,12 @@
     <t xml:space="preserve">https://doi.org/10.34726/hss.2022.79705</t>
   </si>
   <si>
+    <t xml:space="preserve">Nikolas Alge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Profiling of Machine Learning Accelerators using MLPerf</t>
+  </si>
+  <si>
     <t xml:space="preserve">Embedded Machine Learning Scripts and Guides</t>
   </si>
   <si>
@@ -2774,15 +2780,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0\ %"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0"/>
-    <numFmt numFmtId="169" formatCode="dd/mmm"/>
+    <numFmt numFmtId="169" formatCode="DD/MMM"/>
     <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="General"/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -4742,7 +4747,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4758,7 +4763,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4830,6 +4835,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="34" fillId="0" borderId="60" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4874,19 +4883,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="1222">
     <dxf>
@@ -14290,7 +14295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14304,7 +14309,7 @@
       <selection pane="bottomRight" activeCell="B134" activeCellId="0" sqref="B134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.11"/>
@@ -14324,7 +14329,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="4" width="3.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="38" min="32" style="2" width="3.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="39" min="39" style="5" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="40" min="40" style="5" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="40" min="40" style="5" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="41" min="41" style="6" width="7.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="6" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="7" width="38.66"/>
@@ -14333,13 +14338,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="8" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="7" width="35.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="7" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="7" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="7" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="7" width="47.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="7" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="7" width="52.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="7" width="72.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="8.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="55" style="1" width="11.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="55" style="1" width="11.44"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36358,7 +36363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -36368,14 +36373,15 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.56640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="54.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="24.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="10"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="230" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="230" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" s="233" customFormat="true" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37343,26 +37349,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.56640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="22.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="60.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="15.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="247" width="37.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="248" width="11.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="229" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="248" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="229" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" s="250" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37634,13 +37640,27 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
+      <c r="A15" s="228" t="s">
+        <v>702</v>
+      </c>
+      <c r="B15" s="257" t="s">
+        <v>703</v>
+      </c>
+      <c r="C15" s="229" t="s">
+        <v>675</v>
+      </c>
+      <c r="D15" s="229" t="s">
+        <v>671</v>
+      </c>
+      <c r="E15" s="229" t="n">
+        <v>2022</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="256"/>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="257"/>
+      <c r="A18" s="258"/>
     </row>
     <row r="25" s="246" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="245"/>
@@ -37665,7 +37685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -37675,89 +37695,89 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.56640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="229" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="56.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="230" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="230" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="261" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="258" t="s">
+    <row r="1" s="262" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="259" t="s">
         <v>657</v>
       </c>
-      <c r="B1" s="259" t="s">
+      <c r="B1" s="260" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="260" t="s">
+      <c r="C1" s="261" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="245" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B2" s="246" t="s">
-        <v>703</v>
-      </c>
-      <c r="C2" s="262" t="s">
-        <v>704</v>
+        <v>705</v>
+      </c>
+      <c r="C2" s="263" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="228" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="B3" s="229" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C3" s="255" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="228" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B4" s="229" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="C4" s="255" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="228" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B5" s="229" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C5" s="255" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="228" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B6" s="229" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C6" s="255" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="228" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B7" s="229" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C7" s="255" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37803,7 +37823,7 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="243"/>
       <c r="B18" s="244"/>
-      <c r="C18" s="263"/>
+      <c r="C18" s="264"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="246"/>
@@ -37830,288 +37850,266 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="50.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="257" width="50.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="264" t="s">
+      <c r="A1" s="265" t="s">
         <v>659</v>
       </c>
-      <c r="B1" s="264" t="s">
-        <v>720</v>
-      </c>
-      <c r="C1" s="264" t="s">
-        <v>721</v>
-      </c>
-      <c r="D1" s="264" t="s">
+      <c r="B1" s="265" t="s">
         <v>722</v>
       </c>
-      <c r="E1" s="264" t="s">
+      <c r="C1" s="265" t="s">
         <v>723</v>
       </c>
-      <c r="F1" s="264" t="s">
+      <c r="D1" s="265" t="s">
+        <v>724</v>
+      </c>
+      <c r="E1" s="265" t="s">
+        <v>725</v>
+      </c>
+      <c r="F1" s="265" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="264" t="s">
-        <v>724</v>
-      </c>
-      <c r="B2" s="264" t="s">
-        <v>725</v>
-      </c>
-      <c r="C2" s="264" t="s">
+      <c r="A2" s="265" t="s">
         <v>726</v>
       </c>
-      <c r="D2" s="265" t="n">
+      <c r="B2" s="265" t="s">
+        <v>727</v>
+      </c>
+      <c r="C2" s="265" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2" s="266" t="n">
         <v>44562</v>
       </c>
-      <c r="E2" s="266" t="s">
-        <v>727</v>
-      </c>
-      <c r="F2" s="264" t="s">
-        <v>728</v>
+      <c r="E2" s="267" t="s">
+        <v>729</v>
+      </c>
+      <c r="F2" s="265" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="264" t="s">
-        <v>724</v>
-      </c>
-      <c r="B3" s="264" t="s">
-        <v>725</v>
-      </c>
-      <c r="C3" s="264" t="s">
+      <c r="A3" s="265" t="s">
         <v>726</v>
       </c>
-      <c r="D3" s="265" t="n">
+      <c r="B3" s="265" t="s">
+        <v>727</v>
+      </c>
+      <c r="C3" s="265" t="s">
+        <v>728</v>
+      </c>
+      <c r="D3" s="266" t="n">
         <v>44266</v>
       </c>
       <c r="E3" s="256" t="s">
-        <v>729</v>
-      </c>
-      <c r="F3" s="264" t="s">
-        <v>730</v>
+        <v>731</v>
+      </c>
+      <c r="F3" s="265" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="264" t="s">
-        <v>731</v>
-      </c>
-      <c r="B4" s="264" t="s">
-        <v>725</v>
-      </c>
-      <c r="C4" s="264" t="s">
-        <v>726</v>
-      </c>
-      <c r="D4" s="265" t="n">
+      <c r="A4" s="265" t="s">
+        <v>733</v>
+      </c>
+      <c r="B4" s="265" t="s">
+        <v>727</v>
+      </c>
+      <c r="C4" s="265" t="s">
+        <v>728</v>
+      </c>
+      <c r="D4" s="266" t="n">
         <v>44294</v>
       </c>
       <c r="E4" s="256" t="s">
-        <v>732</v>
-      </c>
-      <c r="F4" s="264" t="s">
-        <v>733</v>
+        <v>734</v>
+      </c>
+      <c r="F4" s="265" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>734</v>
-      </c>
-      <c r="D5" s="265" t="n">
+      <c r="A5" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="B5" s="257" t="s">
+        <v>727</v>
+      </c>
+      <c r="C5" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="D5" s="266" t="n">
         <v>44299</v>
       </c>
-      <c r="E5" s="267" t="s">
-        <v>735</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>736</v>
+      <c r="E5" s="268" t="s">
+        <v>737</v>
+      </c>
+      <c r="F5" s="257" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>734</v>
-      </c>
-      <c r="D6" s="265" t="n">
+      <c r="A6" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="B6" s="257" t="s">
+        <v>727</v>
+      </c>
+      <c r="C6" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="D6" s="266" t="n">
         <v>44102</v>
       </c>
-      <c r="E6" s="267" t="s">
-        <v>737</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>738</v>
+      <c r="E6" s="268" t="s">
+        <v>739</v>
+      </c>
+      <c r="F6" s="257" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>734</v>
-      </c>
-      <c r="D7" s="265" t="n">
+      <c r="A7" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="B7" s="257" t="s">
+        <v>727</v>
+      </c>
+      <c r="C7" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="D7" s="266" t="n">
         <v>44562</v>
       </c>
-      <c r="E7" s="267" t="s">
-        <v>739</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>740</v>
+      <c r="E7" s="268" t="s">
+        <v>741</v>
+      </c>
+      <c r="F7" s="257" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>724</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>734</v>
-      </c>
-      <c r="D8" s="265" t="n">
+      <c r="A8" s="257" t="s">
+        <v>726</v>
+      </c>
+      <c r="B8" s="257" t="s">
+        <v>727</v>
+      </c>
+      <c r="C8" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="D8" s="266" t="n">
         <v>44504</v>
       </c>
-      <c r="E8" s="267" t="s">
-        <v>741</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>742</v>
+      <c r="E8" s="268" t="s">
+        <v>743</v>
+      </c>
+      <c r="F8" s="257" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>743</v>
-      </c>
-      <c r="D9" s="265" t="n">
+      <c r="A9" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="B9" s="257" t="s">
+        <v>727</v>
+      </c>
+      <c r="C9" s="257" t="s">
+        <v>745</v>
+      </c>
+      <c r="D9" s="266" t="n">
         <v>44564</v>
       </c>
-      <c r="E9" s="267" t="s">
-        <v>744</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>745</v>
+      <c r="E9" s="268" t="s">
+        <v>746</v>
+      </c>
+      <c r="F9" s="257" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>746</v>
-      </c>
-      <c r="D10" s="265" t="n">
+      <c r="A10" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="B10" s="257" t="s">
+        <v>727</v>
+      </c>
+      <c r="C10" s="257" t="s">
+        <v>748</v>
+      </c>
+      <c r="D10" s="266" t="n">
         <v>42509</v>
       </c>
-      <c r="E10" s="267" t="s">
-        <v>747</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>748</v>
+      <c r="E10" s="268" t="s">
+        <v>749</v>
+      </c>
+      <c r="F10" s="257" t="s">
+        <v>750</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="D11" s="265" t="n">
+      <c r="A11" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="B11" s="257" t="s">
+        <v>727</v>
+      </c>
+      <c r="D11" s="266" t="n">
         <v>43279</v>
       </c>
-      <c r="E11" s="267" t="s">
-        <v>749</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>750</v>
+      <c r="E11" s="268" t="s">
+        <v>751</v>
+      </c>
+      <c r="F11" s="257" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="D12" s="265" t="n">
+      <c r="A12" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="B12" s="257" t="s">
+        <v>727</v>
+      </c>
+      <c r="D12" s="266" t="n">
         <v>43279</v>
       </c>
-      <c r="E12" s="267" t="s">
-        <v>751</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="268"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="268"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="268"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="268"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="268"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="268"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="268"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="268"/>
+      <c r="E12" s="268" t="s">
+        <v>753</v>
+      </c>
+      <c r="F12" s="257" t="s">
+        <v>754</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update Readme and all opentheses from 2021 and 2022
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -14353,7 +14353,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="4" min="3" style="1" width="3.28"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="6" min="5" style="2" width="3.86"/>
@@ -14372,13 +14372,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="38" min="32" style="2" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="39" min="39" style="5" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="40" min="40" style="5" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="41" min="41" style="6" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="41" min="41" style="6" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="6" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="7" width="38.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="7" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="8" width="41.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="8" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="8" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="7" width="35.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="7" width="35.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="7" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="7" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="7" width="47.43"/>
@@ -37909,11 +37909,11 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="10"/>
@@ -37940,7 +37940,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="269" t="s">
         <v>729</v>
       </c>
@@ -37951,7 +37951,7 @@
         <v>731</v>
       </c>
       <c r="D2" s="270" t="n">
-        <v>44562</v>
+        <v>44880</v>
       </c>
       <c r="E2" s="271" t="s">
         <v>732</v>
@@ -37960,7 +37960,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="269" t="s">
         <v>729</v>
       </c>
@@ -37971,7 +37971,7 @@
         <v>731</v>
       </c>
       <c r="D3" s="270" t="n">
-        <v>44266</v>
+        <v>44880</v>
       </c>
       <c r="E3" s="256" t="s">
         <v>734</v>
@@ -37980,7 +37980,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="269" t="s">
         <v>736</v>
       </c>
@@ -37991,7 +37991,7 @@
         <v>731</v>
       </c>
       <c r="D4" s="270" t="n">
-        <v>44294</v>
+        <v>44880</v>
       </c>
       <c r="E4" s="256" t="s">
         <v>737</v>
@@ -38000,7 +38000,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="257" t="s">
         <v>736</v>
       </c>
@@ -38011,7 +38011,7 @@
         <v>739</v>
       </c>
       <c r="D5" s="270" t="n">
-        <v>44299</v>
+        <v>44880</v>
       </c>
       <c r="E5" s="272" t="s">
         <v>740</v>
@@ -38040,7 +38040,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="257" t="s">
         <v>736</v>
       </c>
@@ -38051,7 +38051,7 @@
         <v>739</v>
       </c>
       <c r="D7" s="270" t="n">
-        <v>44562</v>
+        <v>44880</v>
       </c>
       <c r="E7" s="272" t="s">
         <v>744</v>
@@ -38060,7 +38060,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="257" t="s">
         <v>729</v>
       </c>
@@ -38071,7 +38071,7 @@
         <v>739</v>
       </c>
       <c r="D8" s="270" t="n">
-        <v>44504</v>
+        <v>44880</v>
       </c>
       <c r="E8" s="272" t="s">
         <v>746</v>
@@ -38080,7 +38080,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="257" t="s">
         <v>736</v>
       </c>
@@ -38091,7 +38091,7 @@
         <v>748</v>
       </c>
       <c r="D9" s="270" t="n">
-        <v>44564</v>
+        <v>44880</v>
       </c>
       <c r="E9" s="272" t="s">
         <v>749</v>
@@ -38161,7 +38161,7 @@
       <c r="B13" s="257" t="s">
         <v>730</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="257" t="s">
         <v>758</v>
       </c>
       <c r="D13" s="270" t="n">
@@ -38170,13 +38170,13 @@
       <c r="E13" s="257" t="s">
         <v>759</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="257" t="s">
         <v>760</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/"/>
+    <hyperlink ref="F13" r:id="rId1" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/analytical_approximation_of_statistical_rounding.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
AJ: Added the link for Nikolas Alge's thesis.
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EML_Tool_WP" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="762">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2621,6 +2621,9 @@
   </si>
   <si>
     <t xml:space="preserve">Power Profiling of Machine Learning Accelerators using MLPerf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.5281/zenodo.7323206</t>
   </si>
   <si>
     <t xml:space="preserve">Blackthorn</t>
@@ -14351,11 +14354,11 @@
       <selection pane="bottomRight" activeCell="B134" activeCellId="0" sqref="B134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.14"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="4" min="3" style="1" width="3.28"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="4" min="3" style="1" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="6" min="5" style="2" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="7" min="7" style="3" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="13" min="8" style="2" width="3.86"/>
@@ -14372,19 +14375,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="38" min="32" style="2" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="39" min="39" style="5" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="40" min="40" style="5" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="41" min="41" style="6" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="41" min="41" style="6" width="7.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="6" width="8.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="7" width="38.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="8" width="41.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="8" width="41.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="8" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="8" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="7" width="35.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="7" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="7" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="7" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="7" width="47.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="7" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="7" width="52.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="7" width="72.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="7" width="72.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="8.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="55" style="1" width="11.43"/>
   </cols>
@@ -36415,11 +36418,11 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="8.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="54.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="10"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="230" width="11.57"/>
@@ -37396,17 +37399,17 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="60.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="60.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="247" width="37.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="248" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="229" width="11.57"/>
@@ -37680,7 +37683,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="228" t="s">
         <v>702</v>
       </c>
@@ -37695,6 +37698,9 @@
       </c>
       <c r="E15" s="229" t="n">
         <v>2022</v>
+      </c>
+      <c r="F15" s="247" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37714,6 +37720,7 @@
     <hyperlink ref="F6" r:id="rId2" display="https://publik.tuwien.ac.at/files/publik_295897.pdf"/>
     <hyperlink ref="F7" r:id="rId3" display="https://publik.tuwien.ac.at/files/publik_295948.pdf"/>
     <hyperlink ref="F9" r:id="rId4" display="https://publik.tuwien.ac.at/files/publik_296007.pdf"/>
+    <hyperlink ref="F15" r:id="rId5" display="https://doi.org/10.5281/zenodo.7323206"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -37736,7 +37743,7 @@
       <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="229" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="39.43"/>
@@ -37757,79 +37764,79 @@
     </row>
     <row r="2" s="266" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="263" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B2" s="264" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C2" s="265" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="75.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="245" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B3" s="246" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C3" s="267" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="228" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B4" s="229" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C4" s="255" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="228" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B5" s="229" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="C5" s="255" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="228" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B6" s="229" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C6" s="255" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="228" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B7" s="229" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C7" s="255" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="228" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B8" s="229" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C8" s="255" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37909,11 +37916,11 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="10"/>
@@ -37925,16 +37932,16 @@
         <v>659</v>
       </c>
       <c r="B1" s="269" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C1" s="269" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="D1" s="269" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="E1" s="269" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F1" s="269" t="s">
         <v>662</v>
@@ -37942,236 +37949,236 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="269" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B2" s="269" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C2" s="269" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D2" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E2" s="271" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="F2" s="269" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="269" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B3" s="269" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C3" s="269" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D3" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E3" s="256" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="F3" s="269" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="269" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B4" s="269" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C4" s="269" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D4" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E4" s="256" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="F4" s="269" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="257" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B5" s="257" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C5" s="257" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D5" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E5" s="272" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="F5" s="257" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="257" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B6" s="257" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C6" s="257" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D6" s="270" t="n">
         <v>44102</v>
       </c>
       <c r="E6" s="272" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="F6" s="257" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="257" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B7" s="257" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C7" s="257" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D7" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E7" s="272" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="F7" s="257" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="257" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B8" s="257" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C8" s="257" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D8" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E8" s="272" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="F8" s="257" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="257" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B9" s="257" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C9" s="257" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D9" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E9" s="272" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="F9" s="257" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="257" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B10" s="257" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C10" s="257" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="D10" s="270" t="n">
         <v>42509</v>
       </c>
       <c r="E10" s="272" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="F10" s="257" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="257" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B11" s="257" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D11" s="270" t="n">
         <v>43279</v>
       </c>
       <c r="E11" s="272" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="F11" s="257" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="257" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B12" s="257" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D12" s="270" t="n">
         <v>43279</v>
       </c>
       <c r="E12" s="272" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="F12" s="257" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="257" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B13" s="257" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C13" s="257" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D13" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E13" s="257" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="F13" s="257" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -38182,8 +38189,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added a bachelor thesis
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="769">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2810,6 +2810,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Rail_Track_Switch_Filter_V01.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adapting a Railroad Anomaly Detector for Embedded Hardware</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/Adapting_a_Railroad_Anomaly_Detector_for_Embedded_Hardware.pdf</t>
   </si>
 </sst>
 </file>
@@ -14369,25 +14375,25 @@
       <selection pane="bottomRight" activeCell="B134" activeCellId="0" sqref="B134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.45703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.09"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="4" min="3" style="1" width="3.27"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="6" min="5" style="2" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="7" min="7" style="3" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="13" min="8" style="2" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="14" min="14" style="3" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="17" min="15" style="2" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="18" min="18" style="3" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="19" min="19" style="2" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="21" min="20" style="3" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="24" min="22" style="2" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="3" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="27" style="2" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="4" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="38" min="32" style="2" width="3.82"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="6" min="5" style="2" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="7" min="7" style="3" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="13" min="8" style="2" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="14" min="14" style="3" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="17" min="15" style="2" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="18" min="18" style="3" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="19" min="19" style="2" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="21" min="20" style="3" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="24" min="22" style="2" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="3" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="27" style="2" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="4" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="38" min="32" style="2" width="3.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="39" min="39" style="5" width="11.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="40" min="40" style="5" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="41" min="41" style="6" width="7.73"/>
@@ -14397,12 +14403,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="8" width="5.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="8" width="6.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="7" width="35.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="7" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="7" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="7" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="7" width="47.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="7" width="11.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="7" width="47.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="7" width="11.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="7" width="52.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="7" width="72.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="7" width="72.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="8.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="55" style="1" width="11.45"/>
   </cols>
@@ -36433,7 +36439,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="54.45"/>
@@ -37418,14 +37424,14 @@
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="22.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="22.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="60.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="8.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="247" width="37.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="229" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="247" width="37.83"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="248" width="11.54"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="229" width="11.54"/>
   </cols>
@@ -37758,10 +37764,10 @@
       <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="229" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="39.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="39.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="56.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="230" width="11.54"/>
   </cols>
@@ -37929,19 +37935,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="257" width="50.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="257" width="55.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="97.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="97.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38218,7 +38224,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="257" t="s">
         <v>737</v>
       </c>
@@ -38238,11 +38244,31 @@
         <v>766</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="257" t="s">
+        <v>730</v>
+      </c>
+      <c r="B16" s="257" t="s">
+        <v>762</v>
+      </c>
+      <c r="C16" s="257"/>
+      <c r="D16" s="270" t="n">
+        <v>44904</v>
+      </c>
+      <c r="E16" s="257" t="s">
+        <v>767</v>
+      </c>
+      <c r="F16" s="265" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F13" r:id="rId1" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/analytical_approximation_of_statistical_rounding.pdf"/>
     <hyperlink ref="F14" r:id="rId2" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Monocular_Depth_Estimation_V01.pdf"/>
     <hyperlink ref="F15" r:id="rId3" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Rail_Track_Switch_Filter_V01.pdf"/>
+    <hyperlink ref="F16" r:id="rId4" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/Adapting_a_Railroad_Anomaly_Detector_for_Embedded_Hardware.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
changed titel to title
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="768">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2696,9 +2696,6 @@
   </si>
   <si>
     <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titel</t>
   </si>
   <si>
     <t xml:space="preserve">BA</t>
@@ -14405,10 +14402,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="7" width="35.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="7" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="7" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="7" width="47.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="7" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="7" width="47.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="7" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="7" width="52.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="7" width="72.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="7" width="72.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="8.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="55" style="1" width="11.45"/>
   </cols>
@@ -37426,7 +37423,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="22.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="228" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="60.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="8.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="229" width="15.45"/>
@@ -37767,7 +37764,7 @@
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="229" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="39.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="229" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="229" width="56.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="230" width="11.54"/>
   </cols>
@@ -37938,10 +37935,10 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="10"/>
@@ -37964,7 +37961,7 @@
         <v>728</v>
       </c>
       <c r="E1" s="269" t="s">
-        <v>729</v>
+        <v>657</v>
       </c>
       <c r="F1" s="269" t="s">
         <v>662</v>
@@ -37972,294 +37969,294 @@
     </row>
     <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="269" t="s">
+        <v>729</v>
+      </c>
+      <c r="B2" s="269" t="s">
         <v>730</v>
       </c>
-      <c r="B2" s="269" t="s">
+      <c r="C2" s="269" t="s">
         <v>731</v>
-      </c>
-      <c r="C2" s="269" t="s">
-        <v>732</v>
       </c>
       <c r="D2" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E2" s="271" t="s">
+        <v>732</v>
+      </c>
+      <c r="F2" s="269" t="s">
         <v>733</v>
-      </c>
-      <c r="F2" s="269" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="269" t="s">
+        <v>729</v>
+      </c>
+      <c r="B3" s="269" t="s">
         <v>730</v>
       </c>
-      <c r="B3" s="269" t="s">
+      <c r="C3" s="269" t="s">
         <v>731</v>
-      </c>
-      <c r="C3" s="269" t="s">
-        <v>732</v>
       </c>
       <c r="D3" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E3" s="256" t="s">
+        <v>734</v>
+      </c>
+      <c r="F3" s="269" t="s">
         <v>735</v>
-      </c>
-      <c r="F3" s="269" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="269" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B4" s="269" t="s">
+        <v>730</v>
+      </c>
+      <c r="C4" s="269" t="s">
         <v>731</v>
-      </c>
-      <c r="C4" s="269" t="s">
-        <v>732</v>
       </c>
       <c r="D4" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E4" s="256" t="s">
+        <v>737</v>
+      </c>
+      <c r="F4" s="269" t="s">
         <v>738</v>
-      </c>
-      <c r="F4" s="269" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B5" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C5" s="257" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D5" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E5" s="272" t="s">
+        <v>740</v>
+      </c>
+      <c r="F5" s="257" t="s">
         <v>741</v>
-      </c>
-      <c r="F5" s="257" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B6" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C6" s="257" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D6" s="270" t="n">
         <v>44102</v>
       </c>
       <c r="E6" s="272" t="s">
+        <v>742</v>
+      </c>
+      <c r="F6" s="257" t="s">
         <v>743</v>
-      </c>
-      <c r="F6" s="257" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B7" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C7" s="257" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D7" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E7" s="272" t="s">
+        <v>744</v>
+      </c>
+      <c r="F7" s="257" t="s">
         <v>745</v>
-      </c>
-      <c r="F7" s="257" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="257" t="s">
+        <v>729</v>
+      </c>
+      <c r="B8" s="257" t="s">
         <v>730</v>
       </c>
-      <c r="B8" s="257" t="s">
-        <v>731</v>
-      </c>
       <c r="C8" s="257" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D8" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E8" s="272" t="s">
+        <v>746</v>
+      </c>
+      <c r="F8" s="257" t="s">
         <v>747</v>
-      </c>
-      <c r="F8" s="257" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B9" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C9" s="257" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D9" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E9" s="272" t="s">
+        <v>749</v>
+      </c>
+      <c r="F9" s="257" t="s">
         <v>750</v>
-      </c>
-      <c r="F9" s="257" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B10" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C10" s="257" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D10" s="270" t="n">
         <v>42509</v>
       </c>
       <c r="E10" s="272" t="s">
+        <v>752</v>
+      </c>
+      <c r="F10" s="257" t="s">
         <v>753</v>
-      </c>
-      <c r="F10" s="257" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B11" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D11" s="270" t="n">
         <v>43279</v>
       </c>
       <c r="E11" s="272" t="s">
+        <v>754</v>
+      </c>
+      <c r="F11" s="257" t="s">
         <v>755</v>
-      </c>
-      <c r="F11" s="257" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B12" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D12" s="270" t="n">
         <v>43279</v>
       </c>
       <c r="E12" s="272" t="s">
+        <v>756</v>
+      </c>
+      <c r="F12" s="257" t="s">
         <v>757</v>
-      </c>
-      <c r="F12" s="257" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B13" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C13" s="257" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D13" s="270" t="n">
         <v>44880</v>
       </c>
       <c r="E13" s="257" t="s">
+        <v>759</v>
+      </c>
+      <c r="F13" s="265" t="s">
         <v>760</v>
-      </c>
-      <c r="F13" s="265" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B14" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C14" s="257" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D14" s="270" t="n">
         <v>44895</v>
       </c>
       <c r="E14" s="257" t="s">
+        <v>762</v>
+      </c>
+      <c r="F14" s="265" t="s">
         <v>763</v>
-      </c>
-      <c r="F14" s="265" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="257" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B15" s="257" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C15" s="257" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D15" s="270" t="n">
         <v>44895</v>
       </c>
       <c r="E15" s="257" t="s">
+        <v>764</v>
+      </c>
+      <c r="F15" s="265" t="s">
         <v>765</v>
-      </c>
-      <c r="F15" s="265" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="257" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B16" s="257" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C16" s="257"/>
       <c r="D16" s="270" t="n">
         <v>44904</v>
       </c>
       <c r="E16" s="257" t="s">
+        <v>766</v>
+      </c>
+      <c r="F16" s="265" t="s">
         <v>767</v>
-      </c>
-      <c r="F16" s="265" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
first test to rebuild the open thesis page / changed the xlsx file
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="777">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2689,6 +2689,12 @@
     <t xml:space="preserve">https://github.com/embedded-machine-learning/MobileNetV3-Segmentation-Keras</t>
   </si>
   <si>
+    <t xml:space="preserve">Email1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Supervisor 1</t>
   </si>
   <si>
@@ -2701,6 +2707,15 @@
     <t xml:space="preserve">BA</t>
   </si>
   <si>
+    <t xml:space="preserve">axel.jantsch@tuwien.ac.at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matthias.wess@tuwien.ac.at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=9078&amp;dsrid=628&amp;thesisId=83155</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jantsch</t>
   </si>
   <si>
@@ -2710,22 +2725,25 @@
     <t xml:space="preserve">Adaptation of a Latency and Power Estimation Model for ARM Processors</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=9078&amp;dsrid=628&amp;thesisId=83155</t>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8615&amp;dsrid=533&amp;thesisId=89084</t>
   </si>
   <si>
     <t xml:space="preserve">Energy Efficient Adaptive Neural Networks for Embedded Hardware</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8615&amp;dsrid=533&amp;thesisId=89084</t>
-  </si>
-  <si>
     <t xml:space="preserve">DA</t>
   </si>
   <si>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8461&amp;dsrid=505&amp;thesisId=89961</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adaptive Neural Network low bit-width Quantization for image classification, object detection and segmentation targeting FPGA</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8461&amp;dsrid=505&amp;thesisId=89961</t>
+    <t xml:space="preserve">martin.lechner@tuwien.ac.at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=9579&amp;dsrid=362&amp;thesisId=90183</t>
   </si>
   <si>
     <t xml:space="preserve">Lechner</t>
@@ -2734,25 +2752,28 @@
     <t xml:space="preserve">Consistent Semantic Segmentation of Video Objects</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=9579&amp;dsrid=362&amp;thesisId=90183</t>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=7234&amp;dsrid=684&amp;thesisId=83157</t>
   </si>
   <si>
     <t xml:space="preserve">Hardware-Aware Pruning of Neural Networks with Intel Distiller</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=7234&amp;dsrid=684&amp;thesisId=83157</t>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=2782&amp;dsrid=203&amp;thesisId=85720</t>
   </si>
   <si>
     <t xml:space="preserve">Optimierung von 3D Convolutions auf Embedded Hardware für autonomes Fahren</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=2782&amp;dsrid=203&amp;thesisId=85720</t>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8201&amp;dsrid=413&amp;thesisId=96423</t>
   </si>
   <si>
     <t xml:space="preserve">Real-time Simultaneous Face Detection and Pose Estimation</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8201&amp;dsrid=413&amp;thesisId=96423</t>
+    <t xml:space="preserve">matthias.bittner@tuwien.ac.at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8384&amp;dsrid=99&amp;thesisId=98360</t>
   </si>
   <si>
     <t xml:space="preserve">Bittner</t>
@@ -2761,7 +2782,10 @@
     <t xml:space="preserve">Vision based workplace safety monitor in an automotive test bench</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=8384&amp;dsrid=99&amp;thesisId=98360</t>
+    <t xml:space="preserve">nima.taherinejad@tuwien.ac.at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=6371&amp;dsrid=717&amp;thesisId=37487</t>
   </si>
   <si>
     <t xml:space="preserve">Nima</t>
@@ -2770,19 +2794,22 @@
     <t xml:space="preserve">Designing an all-digital DLL for an open-source DDR3 controller</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=6371&amp;dsrid=717&amp;thesisId=37487</t>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=2720&amp;dsrid=822&amp;thesisId=57335</t>
   </si>
   <si>
     <t xml:space="preserve">Deep Learning with Reduced Precision Weights</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=2720&amp;dsrid=822&amp;thesisId=57335</t>
+    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=1203&amp;dsrid=744&amp;thesisId=57337</t>
   </si>
   <si>
     <t xml:space="preserve">Embedded Deep Learning Inference with Shift-CNN</t>
   </si>
   <si>
-    <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=1203&amp;dsrid=744&amp;thesisId=57337</t>
+    <t xml:space="preserve">daniel.schnoell@tuwien.ac.at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/analytical_approximation_of_statistical_rounding.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Schnöll</t>
@@ -2791,7 +2818,10 @@
     <t xml:space="preserve">Analytical Approximation of Statistical Rounding</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/analytical_approximation_of_statistical_rounding.pdf</t>
+    <t xml:space="preserve">maximilian.goetzinger@tuwien.ac.at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Monocular_Depth_Estimation_V01.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Götzinger</t>
@@ -2800,19 +2830,16 @@
     <t xml:space="preserve">Monocular Depth Estimation using Self/Semi-Supervised Learning</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Monocular_Depth_Estimation_V01.pdf</t>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Rail_Track_Switch_Filter_V01.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Filtering of Rail-track Switches using Ensemble Learning</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Rail_Track_Switch_Filter_V01.pdf</t>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/Adapting_a_Railroad_Anomaly_Detector_for_Embedded_Hardware.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Adapting a Railroad Anomaly Detector for Embedded Hardware</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/Adapting_a_Railroad_Anomaly_Detector_for_Embedded_Hardware.pdf</t>
   </si>
 </sst>
 </file>
@@ -37932,22 +37959,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="257" width="50.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="257" width="55.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="97.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="257" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="97.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="257" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="257" width="50.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="257" width="55.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="97.1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="269" t="s">
         <v>659</v>
       </c>
@@ -37958,314 +37988,401 @@
         <v>727</v>
       </c>
       <c r="D1" s="269" t="s">
+        <v>662</v>
+      </c>
+      <c r="E1" s="269" t="s">
         <v>728</v>
       </c>
-      <c r="E1" s="269" t="s">
+      <c r="F1" s="269" t="s">
+        <v>729</v>
+      </c>
+      <c r="G1" s="269" t="s">
+        <v>730</v>
+      </c>
+      <c r="H1" s="269" t="s">
         <v>657</v>
       </c>
-      <c r="F1" s="269" t="s">
-        <v>662</v>
-      </c>
     </row>
-    <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="269" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B2" s="269" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C2" s="269" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2" s="269" t="s">
+        <v>734</v>
+      </c>
+      <c r="E2" s="269" t="s">
+        <v>735</v>
+      </c>
+      <c r="F2" s="269" t="s">
+        <v>736</v>
+      </c>
+      <c r="G2" s="270" t="n">
+        <v>44880</v>
+      </c>
+      <c r="H2" s="271" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="269" t="s">
         <v>731</v>
       </c>
-      <c r="D2" s="270" t="n">
+      <c r="B3" s="269" t="s">
+        <v>732</v>
+      </c>
+      <c r="C3" s="269" t="s">
+        <v>733</v>
+      </c>
+      <c r="D3" s="269" t="s">
+        <v>738</v>
+      </c>
+      <c r="E3" s="269" t="s">
+        <v>735</v>
+      </c>
+      <c r="F3" s="269" t="s">
+        <v>736</v>
+      </c>
+      <c r="G3" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="E2" s="271" t="s">
+      <c r="H3" s="256" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="269" t="s">
+        <v>740</v>
+      </c>
+      <c r="B4" s="269" t="s">
         <v>732</v>
       </c>
-      <c r="F2" s="269" t="s">
+      <c r="C4" s="269" t="s">
         <v>733</v>
       </c>
+      <c r="D4" s="269" t="s">
+        <v>741</v>
+      </c>
+      <c r="E4" s="269" t="s">
+        <v>735</v>
+      </c>
+      <c r="F4" s="269" t="s">
+        <v>736</v>
+      </c>
+      <c r="G4" s="270" t="n">
+        <v>44880</v>
+      </c>
+      <c r="H4" s="256" t="s">
+        <v>742</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="269" t="s">
-        <v>729</v>
-      </c>
-      <c r="B3" s="269" t="s">
-        <v>730</v>
-      </c>
-      <c r="C3" s="269" t="s">
-        <v>731</v>
-      </c>
-      <c r="D3" s="270" t="n">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="257" t="s">
+        <v>740</v>
+      </c>
+      <c r="B5" s="257" t="s">
+        <v>732</v>
+      </c>
+      <c r="C5" s="257" t="s">
+        <v>743</v>
+      </c>
+      <c r="D5" s="257" t="s">
+        <v>744</v>
+      </c>
+      <c r="E5" s="257" t="s">
+        <v>735</v>
+      </c>
+      <c r="F5" s="257" t="s">
+        <v>745</v>
+      </c>
+      <c r="G5" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="E3" s="256" t="s">
-        <v>734</v>
-      </c>
-      <c r="F3" s="269" t="s">
+      <c r="H5" s="272" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="257" t="s">
+        <v>740</v>
+      </c>
+      <c r="B6" s="257" t="s">
+        <v>732</v>
+      </c>
+      <c r="C6" s="257" t="s">
+        <v>743</v>
+      </c>
+      <c r="D6" s="257" t="s">
+        <v>747</v>
+      </c>
+      <c r="E6" s="257" t="s">
         <v>735</v>
       </c>
+      <c r="F6" s="257" t="s">
+        <v>745</v>
+      </c>
+      <c r="G6" s="270" t="n">
+        <v>44102</v>
+      </c>
+      <c r="H6" s="272" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="269" t="s">
-        <v>736</v>
-      </c>
-      <c r="B4" s="269" t="s">
-        <v>730</v>
-      </c>
-      <c r="C4" s="269" t="s">
-        <v>731</v>
-      </c>
-      <c r="D4" s="270" t="n">
-        <v>44880</v>
-      </c>
-      <c r="E4" s="256" t="s">
-        <v>737</v>
-      </c>
-      <c r="F4" s="269" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="257" t="s">
-        <v>736</v>
-      </c>
-      <c r="B5" s="257" t="s">
-        <v>730</v>
-      </c>
-      <c r="C5" s="257" t="s">
-        <v>739</v>
-      </c>
-      <c r="D5" s="270" t="n">
-        <v>44880</v>
-      </c>
-      <c r="E5" s="272" t="s">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="257" t="s">
         <v>740</v>
       </c>
-      <c r="F5" s="257" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="257" t="s">
-        <v>736</v>
-      </c>
-      <c r="B6" s="257" t="s">
-        <v>730</v>
-      </c>
-      <c r="C6" s="257" t="s">
-        <v>739</v>
-      </c>
-      <c r="D6" s="270" t="n">
-        <v>44102</v>
-      </c>
-      <c r="E6" s="272" t="s">
-        <v>742</v>
-      </c>
-      <c r="F6" s="257" t="s">
+      <c r="B7" s="257" t="s">
+        <v>732</v>
+      </c>
+      <c r="C7" s="257" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="257" t="s">
-        <v>736</v>
-      </c>
-      <c r="B7" s="257" t="s">
-        <v>730</v>
-      </c>
-      <c r="C7" s="257" t="s">
-        <v>739</v>
-      </c>
-      <c r="D7" s="270" t="n">
-        <v>44880</v>
-      </c>
-      <c r="E7" s="272" t="s">
-        <v>744</v>
+      <c r="D7" s="257" t="s">
+        <v>749</v>
+      </c>
+      <c r="E7" s="257" t="s">
+        <v>735</v>
       </c>
       <c r="F7" s="257" t="s">
         <v>745</v>
       </c>
+      <c r="G7" s="270" t="n">
+        <v>44880</v>
+      </c>
+      <c r="H7" s="272" t="s">
+        <v>750</v>
+      </c>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="257" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B8" s="257" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C8" s="257" t="s">
-        <v>739</v>
-      </c>
-      <c r="D8" s="270" t="n">
+        <v>743</v>
+      </c>
+      <c r="D8" s="257" t="s">
+        <v>751</v>
+      </c>
+      <c r="E8" s="257" t="s">
+        <v>735</v>
+      </c>
+      <c r="F8" s="257" t="s">
+        <v>745</v>
+      </c>
+      <c r="G8" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="E8" s="272" t="s">
-        <v>746</v>
-      </c>
-      <c r="F8" s="257" t="s">
-        <v>747</v>
+      <c r="H8" s="272" t="s">
+        <v>752</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="257" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B9" s="257" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C9" s="257" t="s">
-        <v>748</v>
-      </c>
-      <c r="D9" s="270" t="n">
+        <v>753</v>
+      </c>
+      <c r="D9" s="257" t="s">
+        <v>754</v>
+      </c>
+      <c r="E9" s="257" t="s">
+        <v>735</v>
+      </c>
+      <c r="F9" s="257" t="s">
+        <v>755</v>
+      </c>
+      <c r="G9" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="E9" s="272" t="s">
-        <v>749</v>
-      </c>
-      <c r="F9" s="257" t="s">
-        <v>750</v>
+      <c r="H9" s="272" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="257" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B10" s="257" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C10" s="257" t="s">
-        <v>751</v>
-      </c>
-      <c r="D10" s="270" t="n">
+        <v>757</v>
+      </c>
+      <c r="D10" s="257" t="s">
+        <v>758</v>
+      </c>
+      <c r="E10" s="257" t="s">
+        <v>735</v>
+      </c>
+      <c r="F10" s="257" t="s">
+        <v>759</v>
+      </c>
+      <c r="G10" s="270" t="n">
         <v>42509</v>
       </c>
-      <c r="E10" s="272" t="s">
-        <v>752</v>
-      </c>
-      <c r="F10" s="257" t="s">
-        <v>753</v>
+      <c r="H10" s="272" t="s">
+        <v>760</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="257" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B11" s="257" t="s">
-        <v>730</v>
-      </c>
-      <c r="D11" s="270" t="n">
+        <v>732</v>
+      </c>
+      <c r="D11" s="257" t="s">
+        <v>761</v>
+      </c>
+      <c r="E11" s="257" t="s">
+        <v>735</v>
+      </c>
+      <c r="G11" s="270" t="n">
         <v>43279</v>
       </c>
-      <c r="E11" s="272" t="s">
-        <v>754</v>
-      </c>
-      <c r="F11" s="257" t="s">
-        <v>755</v>
+      <c r="H11" s="272" t="s">
+        <v>762</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="257" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B12" s="257" t="s">
-        <v>730</v>
-      </c>
-      <c r="D12" s="270" t="n">
+        <v>732</v>
+      </c>
+      <c r="D12" s="257" t="s">
+        <v>763</v>
+      </c>
+      <c r="E12" s="257" t="s">
+        <v>735</v>
+      </c>
+      <c r="G12" s="270" t="n">
         <v>43279</v>
       </c>
-      <c r="E12" s="272" t="s">
-        <v>756</v>
-      </c>
-      <c r="F12" s="257" t="s">
-        <v>757</v>
+      <c r="H12" s="272" t="s">
+        <v>764</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="257" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B13" s="257" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C13" s="257" t="s">
-        <v>758</v>
-      </c>
-      <c r="D13" s="270" t="n">
+        <v>765</v>
+      </c>
+      <c r="D13" s="265" t="s">
+        <v>766</v>
+      </c>
+      <c r="E13" s="257" t="s">
+        <v>735</v>
+      </c>
+      <c r="F13" s="257" t="s">
+        <v>767</v>
+      </c>
+      <c r="G13" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="E13" s="257" t="s">
-        <v>759</v>
-      </c>
-      <c r="F13" s="265" t="s">
-        <v>760</v>
+      <c r="H13" s="257" t="s">
+        <v>768</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="257" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B14" s="257" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C14" s="257" t="s">
-        <v>761</v>
-      </c>
-      <c r="D14" s="270" t="n">
+        <v>769</v>
+      </c>
+      <c r="D14" s="265" t="s">
+        <v>770</v>
+      </c>
+      <c r="E14" s="257" t="s">
+        <v>735</v>
+      </c>
+      <c r="F14" s="257" t="s">
+        <v>771</v>
+      </c>
+      <c r="G14" s="270" t="n">
         <v>44895</v>
       </c>
-      <c r="E14" s="257" t="s">
-        <v>762</v>
-      </c>
-      <c r="F14" s="265" t="s">
-        <v>763</v>
+      <c r="H14" s="257" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="257" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B15" s="257" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C15" s="257" t="s">
-        <v>761</v>
-      </c>
-      <c r="D15" s="270" t="n">
+        <v>769</v>
+      </c>
+      <c r="D15" s="265" t="s">
+        <v>773</v>
+      </c>
+      <c r="E15" s="257" t="s">
+        <v>735</v>
+      </c>
+      <c r="F15" s="257" t="s">
+        <v>771</v>
+      </c>
+      <c r="G15" s="270" t="n">
         <v>44895</v>
       </c>
-      <c r="E15" s="257" t="s">
-        <v>764</v>
-      </c>
-      <c r="F15" s="265" t="s">
-        <v>765</v>
+      <c r="H15" s="257" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="257" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B16" s="257" t="s">
-        <v>761</v>
-      </c>
-      <c r="C16" s="257"/>
-      <c r="D16" s="270" t="n">
+        <v>769</v>
+      </c>
+      <c r="D16" s="265" t="s">
+        <v>775</v>
+      </c>
+      <c r="E16" s="257" t="s">
+        <v>771</v>
+      </c>
+      <c r="F16" s="257"/>
+      <c r="G16" s="270" t="n">
         <v>44904</v>
       </c>
-      <c r="E16" s="257" t="s">
-        <v>766</v>
-      </c>
-      <c r="F16" s="265" t="s">
-        <v>767</v>
+      <c r="H16" s="257" t="s">
+        <v>776</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/analytical_approximation_of_statistical_rounding.pdf"/>
-    <hyperlink ref="F14" r:id="rId2" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Monocular_Depth_Estimation_V01.pdf"/>
-    <hyperlink ref="F15" r:id="rId3" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Rail_Track_Switch_Filter_V01.pdf"/>
-    <hyperlink ref="F16" r:id="rId4" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/Adapting_a_Railroad_Anomaly_Detector_for_Embedded_Hardware.pdf"/>
+    <hyperlink ref="B2" r:id="rId1" display="axel.jantsch@tuwien.ac.at"/>
+    <hyperlink ref="D13" r:id="rId2" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/analytical_approximation_of_statistical_rounding.pdf"/>
+    <hyperlink ref="D14" r:id="rId3" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Monocular_Depth_Estimation_V01.pdf"/>
+    <hyperlink ref="D15" r:id="rId4" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Rail_Track_Switch_Filter_V01.pdf"/>
+    <hyperlink ref="D16" r:id="rId5" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/Adapting_a_Railroad_Anomaly_Detector_for_Embedded_Hardware.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added one master thesis topic
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="779">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2841,12 +2841,18 @@
   <si>
     <t xml:space="preserve">Adapting a Railroad Anomaly Detector for Embedded Hardware</t>
   </si>
+  <si>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/MSC_Segmentation_Disaster.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploring FPGA and eGPU for Disaster-Scene Analysis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0\ %"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
@@ -2855,8 +2861,9 @@
     <numFmt numFmtId="169" formatCode="dd/mmm"/>
     <numFmt numFmtId="170" formatCode="0.0000"/>
     <numFmt numFmtId="171" formatCode="General"/>
+    <numFmt numFmtId="172" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3112,6 +3119,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3880,7 +3893,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="273">
+  <cellXfs count="275">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4973,6 +4986,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -37959,13 +37980,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="257" width="32"/>
@@ -38374,6 +38395,32 @@
       </c>
       <c r="H16" s="257" t="s">
         <v>776</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="257" t="s">
+        <v>740</v>
+      </c>
+      <c r="B17" s="257" t="s">
+        <v>732</v>
+      </c>
+      <c r="C17" s="273" t="s">
+        <v>733</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>777</v>
+      </c>
+      <c r="E17" s="269" t="s">
+        <v>735</v>
+      </c>
+      <c r="F17" s="269" t="s">
+        <v>736</v>
+      </c>
+      <c r="G17" s="274" t="n">
+        <v>44566</v>
+      </c>
+      <c r="H17" s="257" t="s">
+        <v>778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected date field of last entered open thesis
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -2852,7 +2852,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0\ %"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
@@ -2861,9 +2861,8 @@
     <numFmt numFmtId="169" formatCode="dd/mmm"/>
     <numFmt numFmtId="170" formatCode="0.0000"/>
     <numFmt numFmtId="171" formatCode="General"/>
-    <numFmt numFmtId="172" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3119,12 +3118,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3893,7 +3886,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="275">
+  <cellXfs count="273">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4986,14 +4979,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -37983,10 +37968,10 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="257" width="32"/>
@@ -38404,7 +38389,7 @@
       <c r="B17" s="257" t="s">
         <v>732</v>
       </c>
-      <c r="C17" s="273" t="s">
+      <c r="C17" s="257" t="s">
         <v>733</v>
       </c>
       <c r="D17" s="0" t="s">
@@ -38416,7 +38401,7 @@
       <c r="F17" s="269" t="s">
         <v>736</v>
       </c>
-      <c r="G17" s="274" t="n">
+      <c r="G17" s="270" t="n">
         <v>44566</v>
       </c>
       <c r="H17" s="257" t="s">

</xml_diff>

<commit_message>
changed/repaired date of last open thesis
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -37968,14 +37968,15 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="257" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="97.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="36.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="257" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="125.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="257" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="257" width="50.55"/>
@@ -38392,17 +38393,17 @@
       <c r="C17" s="257" t="s">
         <v>733</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="265" t="s">
         <v>777</v>
       </c>
-      <c r="E17" s="269" t="s">
+      <c r="E17" s="257" t="s">
         <v>735</v>
       </c>
-      <c r="F17" s="269" t="s">
+      <c r="F17" s="257" t="s">
         <v>736</v>
       </c>
       <c r="G17" s="270" t="n">
-        <v>44566</v>
+        <v>44931</v>
       </c>
       <c r="H17" s="257" t="s">
         <v>778</v>

</xml_diff>

<commit_message>
removed one open thesis (changed date so that it moves to old open theses)
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -37967,11 +37967,11 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="36.68"/>
@@ -38212,7 +38212,7 @@
         <v>755</v>
       </c>
       <c r="G9" s="270" t="n">
-        <v>44880</v>
+        <v>44515</v>
       </c>
       <c r="H9" s="272" t="s">
         <v>756</v>

</xml_diff>

<commit_message>
added a availibility row in CDLEML_WP_Progress_EML-Process.xlsx nad opentheses.md
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="780">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2689,6 +2689,9 @@
     <t xml:space="preserve">https://github.com/embedded-machine-learning/MobileNetV3-Segmentation-Keras</t>
   </si>
   <si>
+    <t xml:space="preserve">Available</t>
+  </si>
+  <si>
     <t xml:space="preserve">Email1</t>
   </si>
   <si>
@@ -2788,7 +2791,7 @@
     <t xml:space="preserve">https://tiss.tuwien.ac.at/thesis/thesisDetails.xhtml?dswid=6371&amp;dsrid=717&amp;thesisId=37487</t>
   </si>
   <si>
-    <t xml:space="preserve">Nima</t>
+    <t xml:space="preserve">Taherinejad</t>
   </si>
   <si>
     <t xml:space="preserve">Designing an all-digital DLL for an open-source DDR3 controller</t>
@@ -2862,7 +2865,7 @@
     <numFmt numFmtId="170" formatCode="0.0000"/>
     <numFmt numFmtId="171" formatCode="General"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3118,6 +3121,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3886,7 +3895,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="273">
+  <cellXfs count="274">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4979,6 +4988,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -37965,40 +37978,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="257" width="5.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="36.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="257" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="125.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="257" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="257" width="50.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="257" width="55.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="97.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="5.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="257" width="36.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="257" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="125.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="257" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="257" width="50.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="257" width="55.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="97.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="269" t="s">
+      <c r="A1" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="B1" s="269" t="s">
         <v>659</v>
-      </c>
-      <c r="B1" s="269" t="s">
-        <v>726</v>
       </c>
       <c r="C1" s="269" t="s">
         <v>727</v>
       </c>
       <c r="D1" s="269" t="s">
+        <v>728</v>
+      </c>
+      <c r="E1" s="269" t="s">
         <v>662</v>
-      </c>
-      <c r="E1" s="269" t="s">
-        <v>728</v>
       </c>
       <c r="F1" s="269" t="s">
         <v>729</v>
@@ -38007,12 +38021,15 @@
         <v>730</v>
       </c>
       <c r="H1" s="269" t="s">
+        <v>731</v>
+      </c>
+      <c r="I1" s="269" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="269" t="s">
-        <v>731</v>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="269" t="s">
         <v>732</v>
@@ -38029,16 +38046,19 @@
       <c r="F2" s="269" t="s">
         <v>736</v>
       </c>
-      <c r="G2" s="270" t="n">
+      <c r="G2" s="269" t="s">
+        <v>737</v>
+      </c>
+      <c r="H2" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="H2" s="271" t="s">
-        <v>737</v>
+      <c r="I2" s="271" t="s">
+        <v>738</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="269" t="s">
-        <v>731</v>
+    <row r="3" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B3" s="269" t="s">
         <v>732</v>
@@ -38047,375 +38067,420 @@
         <v>733</v>
       </c>
       <c r="D3" s="269" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="E3" s="269" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="F3" s="269" t="s">
         <v>736</v>
       </c>
-      <c r="G3" s="270" t="n">
+      <c r="G3" s="269" t="s">
+        <v>737</v>
+      </c>
+      <c r="H3" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="H3" s="256" t="s">
-        <v>739</v>
+      <c r="I3" s="256" t="s">
+        <v>740</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="269" t="s">
-        <v>740</v>
+    <row r="4" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B4" s="269" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C4" s="269" t="s">
         <v>733</v>
       </c>
       <c r="D4" s="269" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
       <c r="E4" s="269" t="s">
-        <v>735</v>
+        <v>742</v>
       </c>
       <c r="F4" s="269" t="s">
         <v>736</v>
       </c>
-      <c r="G4" s="270" t="n">
+      <c r="G4" s="269" t="s">
+        <v>737</v>
+      </c>
+      <c r="H4" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="H4" s="256" t="s">
-        <v>742</v>
+      <c r="I4" s="256" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="257" t="s">
-        <v>740</v>
+      <c r="A5" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B5" s="257" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C5" s="257" t="s">
-        <v>743</v>
+        <v>733</v>
       </c>
       <c r="D5" s="257" t="s">
         <v>744</v>
       </c>
       <c r="E5" s="257" t="s">
-        <v>735</v>
+        <v>745</v>
       </c>
       <c r="F5" s="257" t="s">
-        <v>745</v>
-      </c>
-      <c r="G5" s="270" t="n">
+        <v>736</v>
+      </c>
+      <c r="G5" s="257" t="s">
+        <v>746</v>
+      </c>
+      <c r="H5" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="H5" s="272" t="s">
-        <v>746</v>
+      <c r="I5" s="272" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="257" t="s">
-        <v>740</v>
+      <c r="A6" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="B6" s="257" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C6" s="257" t="s">
-        <v>743</v>
+        <v>733</v>
       </c>
       <c r="D6" s="257" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="E6" s="257" t="s">
-        <v>735</v>
+        <v>748</v>
       </c>
       <c r="F6" s="257" t="s">
-        <v>745</v>
-      </c>
-      <c r="G6" s="270" t="n">
+        <v>736</v>
+      </c>
+      <c r="G6" s="257" t="s">
+        <v>746</v>
+      </c>
+      <c r="H6" s="270" t="n">
         <v>44102</v>
       </c>
-      <c r="H6" s="272" t="s">
-        <v>748</v>
+      <c r="I6" s="272" t="s">
+        <v>749</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="257" t="s">
-        <v>740</v>
+    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B7" s="257" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C7" s="257" t="s">
-        <v>743</v>
+        <v>733</v>
       </c>
       <c r="D7" s="257" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="E7" s="257" t="s">
-        <v>735</v>
+        <v>750</v>
       </c>
       <c r="F7" s="257" t="s">
-        <v>745</v>
-      </c>
-      <c r="G7" s="270" t="n">
+        <v>736</v>
+      </c>
+      <c r="G7" s="257" t="s">
+        <v>746</v>
+      </c>
+      <c r="H7" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="H7" s="272" t="s">
-        <v>750</v>
+      <c r="I7" s="272" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="257" t="s">
-        <v>731</v>
+      <c r="A8" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B8" s="257" t="s">
         <v>732</v>
       </c>
       <c r="C8" s="257" t="s">
-        <v>743</v>
+        <v>733</v>
       </c>
       <c r="D8" s="257" t="s">
-        <v>751</v>
+        <v>744</v>
       </c>
       <c r="E8" s="257" t="s">
-        <v>735</v>
+        <v>752</v>
       </c>
       <c r="F8" s="257" t="s">
-        <v>745</v>
-      </c>
-      <c r="G8" s="270" t="n">
+        <v>736</v>
+      </c>
+      <c r="G8" s="257" t="s">
+        <v>746</v>
+      </c>
+      <c r="H8" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="H8" s="272" t="s">
-        <v>752</v>
+      <c r="I8" s="272" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="257" t="s">
-        <v>740</v>
+      <c r="A9" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="B9" s="257" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C9" s="257" t="s">
-        <v>753</v>
+        <v>733</v>
       </c>
       <c r="D9" s="257" t="s">
         <v>754</v>
       </c>
       <c r="E9" s="257" t="s">
-        <v>735</v>
+        <v>755</v>
       </c>
       <c r="F9" s="257" t="s">
-        <v>755</v>
-      </c>
-      <c r="G9" s="270" t="n">
-        <v>44515</v>
-      </c>
-      <c r="H9" s="272" t="s">
+        <v>736</v>
+      </c>
+      <c r="G9" s="257" t="s">
         <v>756</v>
+      </c>
+      <c r="H9" s="270" t="n">
+        <v>44880</v>
+      </c>
+      <c r="I9" s="272" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="257" t="s">
-        <v>740</v>
+      <c r="A10" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="B10" s="257" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C10" s="257" t="s">
-        <v>757</v>
+        <v>733</v>
       </c>
       <c r="D10" s="257" t="s">
         <v>758</v>
       </c>
       <c r="E10" s="257" t="s">
-        <v>735</v>
+        <v>759</v>
       </c>
       <c r="F10" s="257" t="s">
-        <v>759</v>
-      </c>
-      <c r="G10" s="270" t="n">
+        <v>736</v>
+      </c>
+      <c r="G10" s="273" t="s">
+        <v>760</v>
+      </c>
+      <c r="H10" s="270" t="n">
         <v>42509</v>
       </c>
-      <c r="H10" s="272" t="s">
-        <v>760</v>
+      <c r="I10" s="272" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="257" t="s">
-        <v>740</v>
+      <c r="A11" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="B11" s="257" t="s">
-        <v>732</v>
-      </c>
-      <c r="D11" s="257" t="s">
-        <v>761</v>
+        <v>741</v>
+      </c>
+      <c r="C11" s="257" t="s">
+        <v>733</v>
       </c>
       <c r="E11" s="257" t="s">
-        <v>735</v>
-      </c>
-      <c r="G11" s="270" t="n">
+        <v>762</v>
+      </c>
+      <c r="F11" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="H11" s="270" t="n">
         <v>43279</v>
       </c>
-      <c r="H11" s="272" t="s">
-        <v>762</v>
+      <c r="I11" s="272" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="257" t="s">
-        <v>740</v>
+      <c r="A12" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="B12" s="257" t="s">
-        <v>732</v>
-      </c>
-      <c r="D12" s="257" t="s">
-        <v>763</v>
+        <v>741</v>
+      </c>
+      <c r="C12" s="257" t="s">
+        <v>733</v>
       </c>
       <c r="E12" s="257" t="s">
-        <v>735</v>
-      </c>
-      <c r="G12" s="270" t="n">
+        <v>764</v>
+      </c>
+      <c r="F12" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="H12" s="270" t="n">
         <v>43279</v>
       </c>
-      <c r="H12" s="272" t="s">
-        <v>764</v>
+      <c r="I12" s="272" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="257" t="s">
-        <v>740</v>
+      <c r="A13" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B13" s="257" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C13" s="257" t="s">
-        <v>765</v>
-      </c>
-      <c r="D13" s="265" t="s">
+        <v>733</v>
+      </c>
+      <c r="D13" s="257" t="s">
         <v>766</v>
       </c>
-      <c r="E13" s="257" t="s">
-        <v>735</v>
+      <c r="E13" s="265" t="s">
+        <v>767</v>
       </c>
       <c r="F13" s="257" t="s">
-        <v>767</v>
-      </c>
-      <c r="G13" s="270" t="n">
+        <v>736</v>
+      </c>
+      <c r="G13" s="257" t="s">
+        <v>768</v>
+      </c>
+      <c r="H13" s="270" t="n">
         <v>44880</v>
       </c>
-      <c r="H13" s="257" t="s">
-        <v>768</v>
+      <c r="I13" s="257" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="257" t="s">
-        <v>740</v>
+      <c r="A14" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B14" s="257" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C14" s="257" t="s">
-        <v>769</v>
-      </c>
-      <c r="D14" s="265" t="s">
+        <v>733</v>
+      </c>
+      <c r="D14" s="257" t="s">
         <v>770</v>
       </c>
-      <c r="E14" s="257" t="s">
-        <v>735</v>
+      <c r="E14" s="265" t="s">
+        <v>771</v>
       </c>
       <c r="F14" s="257" t="s">
-        <v>771</v>
-      </c>
-      <c r="G14" s="270" t="n">
+        <v>736</v>
+      </c>
+      <c r="G14" s="257" t="s">
+        <v>772</v>
+      </c>
+      <c r="H14" s="270" t="n">
         <v>44895</v>
       </c>
-      <c r="H14" s="257" t="s">
-        <v>772</v>
+      <c r="I14" s="257" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="257" t="s">
-        <v>740</v>
+      <c r="A15" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B15" s="257" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C15" s="257" t="s">
-        <v>769</v>
-      </c>
-      <c r="D15" s="265" t="s">
-        <v>773</v>
-      </c>
-      <c r="E15" s="257" t="s">
-        <v>735</v>
+        <v>733</v>
+      </c>
+      <c r="D15" s="257" t="s">
+        <v>770</v>
+      </c>
+      <c r="E15" s="265" t="s">
+        <v>774</v>
       </c>
       <c r="F15" s="257" t="s">
-        <v>771</v>
-      </c>
-      <c r="G15" s="270" t="n">
+        <v>736</v>
+      </c>
+      <c r="G15" s="257" t="s">
+        <v>772</v>
+      </c>
+      <c r="H15" s="270" t="n">
         <v>44895</v>
       </c>
-      <c r="H15" s="257" t="s">
-        <v>774</v>
+      <c r="I15" s="257" t="s">
+        <v>775</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="257" t="s">
-        <v>731</v>
+      <c r="A16" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B16" s="257" t="s">
-        <v>769</v>
-      </c>
-      <c r="D16" s="265" t="s">
-        <v>775</v>
-      </c>
-      <c r="E16" s="257" t="s">
-        <v>771</v>
-      </c>
-      <c r="F16" s="257"/>
-      <c r="G16" s="270" t="n">
+        <v>732</v>
+      </c>
+      <c r="C16" s="257" t="s">
+        <v>770</v>
+      </c>
+      <c r="E16" s="265" t="s">
+        <v>776</v>
+      </c>
+      <c r="F16" s="257" t="s">
+        <v>772</v>
+      </c>
+      <c r="G16" s="257"/>
+      <c r="H16" s="270" t="n">
         <v>44904</v>
       </c>
-      <c r="H16" s="257" t="s">
-        <v>776</v>
+      <c r="I16" s="257" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="257" t="s">
-        <v>740</v>
+      <c r="A17" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B17" s="257" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C17" s="257" t="s">
         <v>733</v>
       </c>
-      <c r="D17" s="265" t="s">
-        <v>777</v>
-      </c>
-      <c r="E17" s="257" t="s">
-        <v>735</v>
+      <c r="D17" s="257" t="s">
+        <v>734</v>
+      </c>
+      <c r="E17" s="265" t="s">
+        <v>778</v>
       </c>
       <c r="F17" s="257" t="s">
         <v>736</v>
       </c>
-      <c r="G17" s="270" t="n">
+      <c r="G17" s="257" t="s">
+        <v>737</v>
+      </c>
+      <c r="H17" s="270" t="n">
         <v>44931</v>
       </c>
-      <c r="H17" s="257" t="s">
-        <v>778</v>
+      <c r="I17" s="257" t="s">
+        <v>779</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="axel.jantsch@tuwien.ac.at"/>
-    <hyperlink ref="D13" r:id="rId2" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/analytical_approximation_of_statistical_rounding.pdf"/>
-    <hyperlink ref="D14" r:id="rId3" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Monocular_Depth_Estimation_V01.pdf"/>
-    <hyperlink ref="D15" r:id="rId4" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Rail_Track_Switch_Filter_V01.pdf"/>
-    <hyperlink ref="D16" r:id="rId5" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/Adapting_a_Railroad_Anomaly_Detector_for_Embedded_Hardware.pdf"/>
+    <hyperlink ref="C2" r:id="rId1" display="axel.jantsch@tuwien.ac.at"/>
+    <hyperlink ref="E13" r:id="rId2" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/analytical_approximation_of_statistical_rounding.pdf"/>
+    <hyperlink ref="E14" r:id="rId3" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Monocular_Depth_Estimation_V01.pdf"/>
+    <hyperlink ref="E15" r:id="rId4" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Rail_Track_Switch_Filter_V01.pdf"/>
+    <hyperlink ref="E16" r:id="rId5" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/Adapting_a_Railroad_Anomaly_Detector_for_Embedded_Hardware.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added 4 new theses
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="788">
   <si>
     <t xml:space="preserve">Compliance zu WPs CDLEML</t>
   </si>
@@ -2850,6 +2850,30 @@
   <si>
     <t xml:space="preserve">Exploring FPGA and eGPU for Disaster-Scene Analysis</t>
   </si>
+  <si>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/EMLCDL_Master_Depth-wiseConcatenationOfTwoPrunedNetworks_V01.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth-wise Concatenation of Two Pruned Networks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/EMLCDL_Master_EvaluationOfLaneDetectionCNNsForRailTracks.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluation of Lane Detection CNNs for Rail Tracks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/EMLCDL_Master_ReinforcementLearningForTrainRoutePrediction.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reinforcement Learning for Train Route Prediction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://eml.ict.tuwien.ac.at/PublFiles/Theses/EMLCDL_Master_SimultaneousDetectionAndSegmentationOfDifferentObjects.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simultaneous Detection and Segmentation of Different Objects</t>
+  </si>
 </sst>
 </file>
 
@@ -2865,7 +2889,7 @@
     <numFmt numFmtId="170" formatCode="0.0000"/>
     <numFmt numFmtId="171" formatCode="General"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3121,12 +3145,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3895,7 +3913,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="274">
+  <cellXfs count="273">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4988,10 +5006,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -37978,13 +37992,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="5.09"/>
@@ -38278,7 +38292,7 @@
       <c r="F10" s="257" t="s">
         <v>736</v>
       </c>
-      <c r="G10" s="273" t="s">
+      <c r="G10" s="257" t="s">
         <v>760</v>
       </c>
       <c r="H10" s="270" t="n">
@@ -38472,6 +38486,122 @@
       </c>
       <c r="I17" s="257" t="s">
         <v>779</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="257" t="s">
+        <v>741</v>
+      </c>
+      <c r="C18" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="D18" s="257" t="s">
+        <v>770</v>
+      </c>
+      <c r="E18" s="265" t="s">
+        <v>780</v>
+      </c>
+      <c r="F18" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="G18" s="257" t="s">
+        <v>772</v>
+      </c>
+      <c r="H18" s="270" t="n">
+        <v>45113</v>
+      </c>
+      <c r="I18" s="257" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="257" t="s">
+        <v>741</v>
+      </c>
+      <c r="C19" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="D19" s="257" t="s">
+        <v>770</v>
+      </c>
+      <c r="E19" s="265" t="s">
+        <v>782</v>
+      </c>
+      <c r="F19" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="G19" s="257" t="s">
+        <v>772</v>
+      </c>
+      <c r="H19" s="270" t="n">
+        <v>45113</v>
+      </c>
+      <c r="I19" s="257" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="257" t="s">
+        <v>741</v>
+      </c>
+      <c r="C20" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="D20" s="257" t="s">
+        <v>770</v>
+      </c>
+      <c r="E20" s="265" t="s">
+        <v>784</v>
+      </c>
+      <c r="F20" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="G20" s="257" t="s">
+        <v>772</v>
+      </c>
+      <c r="H20" s="270" t="n">
+        <v>45113</v>
+      </c>
+      <c r="I20" s="257" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="257" t="s">
+        <v>741</v>
+      </c>
+      <c r="C21" s="257" t="s">
+        <v>733</v>
+      </c>
+      <c r="D21" s="257" t="s">
+        <v>770</v>
+      </c>
+      <c r="E21" s="265" t="s">
+        <v>786</v>
+      </c>
+      <c r="F21" s="257" t="s">
+        <v>736</v>
+      </c>
+      <c r="G21" s="257" t="s">
+        <v>772</v>
+      </c>
+      <c r="H21" s="270" t="n">
+        <v>45113</v>
+      </c>
+      <c r="I21" s="257" t="s">
+        <v>787</v>
       </c>
     </row>
   </sheetData>
@@ -38481,6 +38611,7 @@
     <hyperlink ref="E14" r:id="rId3" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Monocular_Depth_Estimation_V01.pdf"/>
     <hyperlink ref="E15" r:id="rId4" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EML_Master_Thesis_Rail_Track_Switch_Filter_V01.pdf"/>
     <hyperlink ref="E16" r:id="rId5" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/Adapting_a_Railroad_Anomaly_Detector_for_Embedded_Hardware.pdf"/>
+    <hyperlink ref="E18" r:id="rId6" display="https://eml.ict.tuwien.ac.at/PublFiles/Theses/EMLCDL_Master_Depth-wiseConcatenationOfTwoPrunedNetworks_V01.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
try to fix problem with newest 4 theses
</commit_message>
<xml_diff>
--- a/_data/CDLEML_WP_Progress_EML-Process.xlsx
+++ b/_data/CDLEML_WP_Progress_EML-Process.xlsx
@@ -37994,11 +37994,11 @@
   </sheetPr>
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="257" width="5.09"/>
@@ -38511,7 +38511,7 @@
         <v>772</v>
       </c>
       <c r="H18" s="270" t="n">
-        <v>45113</v>
+        <v>45108</v>
       </c>
       <c r="I18" s="257" t="s">
         <v>781</v>
@@ -38540,7 +38540,7 @@
         <v>772</v>
       </c>
       <c r="H19" s="270" t="n">
-        <v>45113</v>
+        <v>45108</v>
       </c>
       <c r="I19" s="257" t="s">
         <v>783</v>
@@ -38569,7 +38569,7 @@
         <v>772</v>
       </c>
       <c r="H20" s="270" t="n">
-        <v>45113</v>
+        <v>45108</v>
       </c>
       <c r="I20" s="257" t="s">
         <v>785</v>
@@ -38598,7 +38598,7 @@
         <v>772</v>
       </c>
       <c r="H21" s="270" t="n">
-        <v>45113</v>
+        <v>45108</v>
       </c>
       <c r="I21" s="257" t="s">
         <v>787</v>

</xml_diff>